<commit_message>
extend tests capture more issues
</commit_message>
<xml_diff>
--- a/tests/v0/data/_schema/physical_invalid/no-container-no-container-property-index-constraints.xlsx
+++ b/tests/v0/data/_schema/physical_invalid/no-container-no-container-property-index-constraints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikola/repos/neat/tests/v0/data/_schema/physical_invalid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E91BF8A-E7E4-B148-B3E0-D40849D6E007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CECE05-626D-4147-89DE-43B5791B666E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="38400" windowHeight="24000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
   <si>
     <t>role</t>
   </si>
@@ -239,10 +239,25 @@
     <t>Some</t>
   </si>
   <si>
-    <t>container</t>
-  </si>
-  <si>
     <t>veryVeryLongIdentifierWhichIsLongerThanMinAllowedNumberOfCharactersveryVeryLongIdentifierWhichIsLongerThanMinAllowedNumberOfCharactersveryVeryLongIdentifierWhichIsLongerThanMinAllowedNumberOfCharactersveryVeryLongIdentifierWhichIsLongerThanMinAllowedNumberOfCharactersveryVeryLongIdentifierWhichIsLongerThanMinAllowedNumberOfCharacters</t>
+  </si>
+  <si>
+    <t>some5</t>
+  </si>
+  <si>
+    <t>property2</t>
+  </si>
+  <si>
+    <t>property1</t>
+  </si>
+  <si>
+    <t>requires:constraint</t>
+  </si>
+  <si>
+    <t>uniqueness:SomeId(container=Some)</t>
+  </si>
+  <si>
+    <t>requires:SomeIdSomeIdSomeIdSomeIdSomeIdSomeIdSomeIdSomeIdSomeIdSomeIdSomeIdSomeIdSomeId(container=Some)</t>
   </si>
 </sst>
 </file>
@@ -745,9 +760,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
+      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -999,32 +1014,50 @@
         <v>65</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="A8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
@@ -4103,11 +4136,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4153,7 +4186,21 @@
       <c r="A3" t="s">
         <v>65</v>
       </c>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
       <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4314,7 +4361,7 @@
       </c>
       <c r="D2" t="str">
         <f>IF(ISBLANK(Containers!A4), "", Containers!A4)</f>
-        <v/>
+        <v>Some</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>

</xml_diff>